<commit_message>
Obtained final signals and started FDA on them
</commit_message>
<xml_diff>
--- a/excels_tsv/Epochs_droppped.xlsx
+++ b/excels_tsv/Epochs_droppped.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/52815a9a376fd39c/Desktop/NL3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\OneDrive\Desktop\NL3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{2B62F507-BDA1-4943-87C6-857E170414DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E81E7DD0-2DAC-49CA-858A-34F705640C41}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86706257-90E4-4FE9-A614-78E638200C6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DE92103D-7851-4A93-AF60-DD8215C82B7B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>% Epochs Dropped</t>
   </si>
@@ -51,6 +51,12 @@
   </si>
   <si>
     <t>FIR</t>
+  </si>
+  <si>
+    <t>AUTOREJECT</t>
+  </si>
+  <si>
+    <t>Threshold</t>
   </si>
 </sst>
 </file>
@@ -94,7 +100,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -102,6 +108,7 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -420,31 +427,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF425CEC-3615-455A-9CD0-FBBCCB549A65}">
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B2" s="5" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C2" s="6"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -454,8 +463,14 @@
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -465,8 +480,14 @@
       <c r="C4" s="2">
         <v>0.108</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="E4">
+        <v>3.2868127119523401E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -476,8 +497,15 @@
       <c r="C5" s="3">
         <v>4.3999999999999997E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1.1354786009950301E-3</v>
+      </c>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -487,8 +515,14 @@
       <c r="C6" s="3">
         <v>0.14699999999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>3.3041984184570801E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>4</v>
       </c>
@@ -498,8 +532,14 @@
       <c r="C7" s="3">
         <v>2E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>2.05740405048585E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>5</v>
       </c>
@@ -509,8 +549,14 @@
       <c r="C8" s="3">
         <v>3.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>1.4738356454772701E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>6</v>
       </c>
@@ -520,8 +566,14 @@
       <c r="C9" s="3">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>1.4314424280611701E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>7</v>
       </c>
@@ -531,8 +583,14 @@
       <c r="C10" s="3">
         <v>0.27800000000000002</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10" s="2">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>5.91921310721786E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>8</v>
       </c>
@@ -542,8 +600,14 @@
       <c r="C11" s="3">
         <v>0.128</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>3.1069460573752601E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>9</v>
       </c>
@@ -553,8 +617,14 @@
       <c r="C12" s="3">
         <v>2.8000000000000001E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E12">
+        <v>5.1330900475964904E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>10</v>
       </c>
@@ -564,8 +634,14 @@
       <c r="C13" s="3">
         <v>0.158</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>5.4487834129254701E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>11</v>
       </c>
@@ -575,8 +651,14 @@
       <c r="C14" s="3">
         <v>0.80700000000000005</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>1.9002787618916501E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>12</v>
       </c>
@@ -586,8 +668,14 @@
       <c r="C15" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D15" s="2">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>4.6730206729784698E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>13</v>
       </c>
@@ -597,8 +685,14 @@
       <c r="C16" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16" s="2">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0.18602805874174599</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>14</v>
       </c>
@@ -608,8 +702,14 @@
       <c r="C17" s="3">
         <v>1.2999999999999999E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="E17" s="5">
+        <v>5.0019790055730198E-5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>15</v>
       </c>
@@ -619,8 +719,14 @@
       <c r="C18" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D18" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="E18">
+        <v>2.3418901681103101E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>16</v>
       </c>
@@ -630,8 +736,14 @@
       <c r="C19" s="3">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D19" s="2">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>2.40286305161034E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>17</v>
       </c>
@@ -641,8 +753,14 @@
       <c r="C20" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D20" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="E20">
+        <v>1.5279868748495401E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>18</v>
       </c>
@@ -652,8 +770,14 @@
       <c r="C21" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D21" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="E21">
+        <v>1.0804329792613501E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>19</v>
       </c>
@@ -663,8 +787,14 @@
       <c r="C22" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D22" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="E22">
+        <v>2.8188762723774302E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>20</v>
       </c>
@@ -674,8 +804,14 @@
       <c r="C23" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D23" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="E23">
+        <v>7.1360624853334905E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>21</v>
       </c>
@@ -685,8 +821,14 @@
       <c r="C24" s="3">
         <v>4.5999999999999999E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D24" s="2">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="E24">
+        <v>1.27985369720505E-4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>22</v>
       </c>
@@ -696,8 +838,14 @@
       <c r="C25" s="4">
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D25" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="E25">
+        <v>5.4443869150731805E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>23</v>
       </c>
@@ -707,8 +855,14 @@
       <c r="C26" s="3">
         <v>0.36299999999999999</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D26" s="2">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>1.0509863830914901E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>24</v>
       </c>
@@ -718,8 +872,14 @@
       <c r="C27" s="3">
         <v>5.8999999999999997E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D27" s="2">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>2.70212461224029E-4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>25</v>
       </c>
@@ -729,8 +889,14 @@
       <c r="C28" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D28" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="E28">
+        <v>9.21856458575309E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>26</v>
       </c>
@@ -740,8 +906,14 @@
       <c r="C29" s="3">
         <v>1.4E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D29" s="2">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>7.76994632038501E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>27</v>
       </c>
@@ -751,8 +923,14 @@
       <c r="C30" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D30" s="2">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>2.9474303542584099E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>28</v>
       </c>
@@ -762,8 +940,14 @@
       <c r="C31" s="3">
         <v>0.25600000000000001</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D31" s="2">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>4.5137187057741398E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>29</v>
       </c>
@@ -773,8 +957,14 @@
       <c r="C32" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D32" s="2">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>9.2237056727030899E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>30</v>
       </c>
@@ -784,8 +974,14 @@
       <c r="C33" s="3">
         <v>0.26800000000000002</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D33" s="2">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>1.6538274595367501E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>31</v>
       </c>
@@ -795,8 +991,11 @@
       <c r="C34" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D34" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>32</v>
       </c>
@@ -806,8 +1005,11 @@
       <c r="C35" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D35" s="2">
+        <v>0.33299999999999996</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>33</v>
       </c>
@@ -817,8 +1019,11 @@
       <c r="C36" s="3">
         <v>3.1E-2</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D36" s="2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>34</v>
       </c>
@@ -828,8 +1033,11 @@
       <c r="C37" s="3">
         <v>2.1000000000000001E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D37" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>35</v>
       </c>
@@ -839,8 +1047,11 @@
       <c r="C38" s="3">
         <v>8.0000000000000002E-3</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D38" s="2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>36</v>
       </c>
@@ -850,8 +1061,11 @@
       <c r="C39" s="3">
         <v>0.93100000000000005</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D39" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>37</v>
       </c>
@@ -861,8 +1075,11 @@
       <c r="C40" s="3">
         <v>0.26700000000000002</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D40" s="3">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>38</v>
       </c>
@@ -872,8 +1089,11 @@
       <c r="C41" s="3">
         <v>0.113</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D41" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>39</v>
       </c>
@@ -883,8 +1103,11 @@
       <c r="C42" s="3">
         <v>0.98499999999999999</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D42" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>40</v>
       </c>
@@ -894,8 +1117,14 @@
       <c r="C43" s="3">
         <v>0.121</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D43" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="E43" s="5">
+        <v>2.9658319767110898E-5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>41</v>
       </c>
@@ -905,8 +1134,14 @@
       <c r="C44" s="3">
         <v>0.308</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D44" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="E44" s="5">
+        <v>2.1335968638865101E-4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>42</v>
       </c>
@@ -916,8 +1151,14 @@
       <c r="C45" s="2">
         <v>0.20200000000000001</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D45" s="3">
+        <v>0</v>
+      </c>
+      <c r="E45" s="5">
+        <v>3.2944759755447199E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>43</v>
       </c>
@@ -927,8 +1168,14 @@
       <c r="C46" s="2">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D46" s="3">
+        <v>0.312</v>
+      </c>
+      <c r="E46" s="5">
+        <v>2.6728403358308402E-4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>44</v>
       </c>
@@ -938,8 +1185,14 @@
       <c r="C47" s="2">
         <v>0.20399999999999999</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D47" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="E47" s="5">
+        <v>3.7365993376928498E-5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>45</v>
       </c>
@@ -949,8 +1202,14 @@
       <c r="C48" s="2">
         <v>0.14399999999999999</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D48" s="3">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>3.3466163271822399E-4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>46</v>
       </c>
@@ -960,8 +1219,14 @@
       <c r="C49" s="2">
         <v>0.28799999999999998</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D49" s="3">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>6.4712009797319298E-4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>47</v>
       </c>
@@ -971,8 +1236,14 @@
       <c r="C50" s="2">
         <v>0.247</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D50" s="3">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>4.8302818035576899E-4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>48</v>
       </c>
@@ -982,8 +1253,14 @@
       <c r="C51" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D51" s="3">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>1.80003919940958E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>49</v>
       </c>
@@ -993,8 +1270,14 @@
       <c r="C52" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D52" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="E52">
+        <v>1.1170761088547801E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>50</v>
       </c>
@@ -1003,6 +1286,12 @@
       </c>
       <c r="C53" s="2">
         <v>0.20699999999999999</v>
+      </c>
+      <c r="D53" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="E53" s="5">
+        <v>6.5361291315035002E-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>